<commit_message>
SDProp implimentation v.0.1 (error fixed)
</commit_message>
<xml_diff>
--- a/ChangeLog.xlsx
+++ b/ChangeLog.xlsx
@@ -968,7 +968,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1110,7 +1110,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1728,14 +1728,6 @@
       <filters blank="1">
         <filter val="○"/>
         <filter val="○コメントアウトしてある"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters blank="1">
-        <filter val="0%"/>
-        <filter val="10%"/>
-        <filter val="5%"/>
-        <filter val="90%"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>